<commit_message>
home filters added and send email functionality as well
</commit_message>
<xml_diff>
--- a/data_exports/enrollments_cleaned_1960586.xlsx
+++ b/data_exports/enrollments_cleaned_1960586.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,13 +539,13 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45848.05543981482</v>
+        <v>45859.62804398148</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1.100277777777778</v>
+        <v>2.118888888888889</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -565,24 +565,24 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>84.21</t>
+          <t>94.72</t>
         </is>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>15.75</t>
+          <t>29.81</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>84.21</t>
+          <t>94.72</t>
         </is>
       </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
-          <t>15.75</t>
+          <t>29.81</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr"/>
@@ -602,13 +602,13 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45848.79341435185</v>
+        <v>45857.81793981481</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>5.013333333333334</v>
+        <v>5.538055555555555</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -628,24 +628,24 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>96.19</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>21.75</t>
+          <t>30.37</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>96.19</t>
         </is>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>21.75</t>
+          <t>30.37</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr"/>
@@ -665,13 +665,13 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45847.80886574074</v>
+        <v>45859.60306712963</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>2.273333333333333</v>
+        <v>2.439166666666666</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -691,24 +691,24 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>83.33</t>
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>17.65</t>
+          <t>23.18</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>83.33</t>
         </is>
       </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
-          <t>17.65</t>
+          <t>23.18</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr"/>
@@ -728,13 +728,13 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45849.62803240741</v>
+        <v>45859.60295138889</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>3.8925</v>
+        <v>4.2325</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -754,24 +754,24 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t>91.70</t>
+          <t>95.89</t>
         </is>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
-          <t>49.62</t>
+          <t>45.68</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>91.70</t>
+          <t>95.89</t>
         </is>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
-          <t>49.62</t>
+          <t>45.68</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr"/>
@@ -791,13 +791,13 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>45847.56543981482</v>
+        <v>45859.59982638889</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5533333333333333</v>
+        <v>0.5927777777777777</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -817,24 +817,24 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>83.48</t>
         </is>
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
-          <t>16.40</t>
+          <t>23.16</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>83.48</t>
         </is>
       </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
-          <t>16.40</t>
+          <t>23.16</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr"/>
@@ -854,13 +854,13 @@
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>45847.6021875</v>
+        <v>45858.66373842592</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1.107222222222222</v>
+        <v>1.819166666666667</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -880,24 +880,24 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>91.15</t>
         </is>
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
-          <t>16.40</t>
+          <t>26.56</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>91.15</t>
         </is>
       </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr">
         <is>
-          <t>16.40</t>
+          <t>26.56</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr"/>
@@ -917,13 +917,13 @@
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>45848.99476851852</v>
+        <v>45859.14892361111</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>2.933611111111111</v>
+        <v>3.723611111111111</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -943,24 +943,24 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>97.39</t>
         </is>
       </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr">
         <is>
-          <t>21.75</t>
+          <t>47.09</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>97.39</t>
         </is>
       </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
         <is>
-          <t>21.75</t>
+          <t>47.09</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr"/>
@@ -980,13 +980,13 @@
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>45848.73710648148</v>
+        <v>45859.09912037037</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1.665555555555555</v>
+        <v>3.1075</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1006,24 +1006,24 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t>77.02</t>
+          <t>41.62</t>
         </is>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
-          <t>13.02</t>
+          <t>18.37</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>77.02</t>
+          <t>41.62</t>
         </is>
       </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
-          <t>13.02</t>
+          <t>18.37</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr"/>
@@ -1043,13 +1043,13 @@
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>45849.63467592592</v>
+        <v>45859.56491898148</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>4.007222222222222</v>
+        <v>5.151666666666666</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1069,24 +1069,24 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>89.97</t>
+          <t>89.13</t>
         </is>
       </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr">
         <is>
-          <t>17.94</t>
+          <t>25.23</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>89.97</t>
+          <t>89.13</t>
         </is>
       </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr">
         <is>
-          <t>17.94</t>
+          <t>25.23</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr"/>
@@ -1106,13 +1106,13 @@
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>45847.59469907408</v>
+        <v>45859.63033564815</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>3.238055555555555</v>
+        <v>5.633055555555556</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1132,24 +1132,24 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t>94.67</t>
+          <t>96.62</t>
         </is>
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr">
         <is>
-          <t>26.29</t>
+          <t>29.31</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>94.67</t>
+          <t>96.62</t>
         </is>
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
-          <t>26.29</t>
+          <t>29.31</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr"/>
@@ -1169,10 +1169,10 @@
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>45849.72796296296</v>
+        <v>45851.76115740741</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>1.399166666666667</v>
@@ -1195,24 +1195,24 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
-          <t>92.42</t>
+          <t>77.04</t>
         </is>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
-          <t>25.63</t>
+          <t>20.63</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>92.42</t>
+          <t>77.04</t>
         </is>
       </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr">
         <is>
-          <t>25.63</t>
+          <t>20.63</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr"/>
@@ -1232,13 +1232,13 @@
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>45849.09577546296</v>
+        <v>45859.62957175926</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>3.904444444444445</v>
+        <v>5.645277777777777</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1258,24 +1258,24 @@
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
-          <t>95.03</t>
+          <t>99.64</t>
         </is>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr">
         <is>
-          <t>24.86</t>
+          <t>34.63</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>95.03</t>
+          <t>99.64</t>
         </is>
       </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr">
         <is>
-          <t>24.86</t>
+          <t>34.63</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr"/>
@@ -1295,13 +1295,13 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>45848.0831712963</v>
+        <v>45859.6199537037</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>1.258333333333333</v>
+        <v>1.905277777777778</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1321,24 +1321,24 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>85.13</t>
+          <t>89.72</t>
         </is>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr">
         <is>
-          <t>16.10</t>
+          <t>24.18</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>85.13</t>
+          <t>89.72</t>
         </is>
       </c>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr">
         <is>
-          <t>16.10</t>
+          <t>24.18</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr"/>
@@ -1358,13 +1358,13 @@
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>45847.81611111111</v>
+        <v>45858.85299768519</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>1.667777777777778</v>
+        <v>2.266111111111111</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1384,24 +1384,24 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>84.45</t>
         </is>
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr">
         <is>
-          <t>16.40</t>
+          <t>24.03</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>84.45</t>
         </is>
       </c>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr">
         <is>
-          <t>16.40</t>
+          <t>24.03</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr"/>
@@ -1421,13 +1421,13 @@
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>45847.56755787037</v>
+        <v>45859.55833333333</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>1.986388888888889</v>
+        <v>2.164444444444444</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1447,24 +1447,24 @@
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>86.30</t>
         </is>
       </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr">
         <is>
-          <t>17.65</t>
+          <t>23.31</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>86.30</t>
         </is>
       </c>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr">
         <is>
-          <t>17.65</t>
+          <t>23.31</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr"/>
@@ -1484,13 +1484,13 @@
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>45849.11145833333</v>
+        <v>45859.61820601852</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>2.840833333333333</v>
+        <v>3.443888888888889</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1510,31 +1510,31 @@
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
-          <t>90.79</t>
+          <t>74.41</t>
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr">
         <is>
-          <t>18.25</t>
+          <t>24.33</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>90.79</t>
+          <t>74.41</t>
         </is>
       </c>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr">
         <is>
-          <t>18.25</t>
+          <t>24.33</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>5447867</v>
+        <v>5459867</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1547,13 +1547,13 @@
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>45848.74724537037</v>
+        <v>45856.20641203703</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
-        <v>1.578055555555556</v>
+        <v>8.928888888888888</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1567,37 +1567,37 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>U79139939</t>
+          <t>U20279434</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>80.50</t>
         </is>
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
-          <t>16.40</t>
+          <t>26.21</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>80.50</t>
         </is>
       </c>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr">
         <is>
-          <t>16.40</t>
+          <t>26.21</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>5476707</v>
+        <v>5447867</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1610,13 +1610,13 @@
         </is>
       </c>
       <c r="D19" s="2" t="n">
-        <v>45847.60293981482</v>
+        <v>45859.6034375</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>16.8825</v>
+        <v>16.40305555555556</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1625,42 +1625,42 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>CGS2100.002U25</t>
+          <t>CGS2100.021U25</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>U56204068</t>
+          <t>U79139939</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
-          <t>90.59</t>
+          <t>86.66</t>
         </is>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr">
         <is>
-          <t>25.71</t>
+          <t>24.97</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>90.59</t>
+          <t>86.66</t>
         </is>
       </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr">
         <is>
-          <t>25.71</t>
+          <t>24.97</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>5446521</v>
+        <v>5476707</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1673,13 +1673,13 @@
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>45848.03944444445</v>
+        <v>45859.62878472222</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>3.073333333333333</v>
+        <v>18.00333333333333</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1688,42 +1688,42 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>CGS2100.021U25</t>
+          <t>CGS2100.002U25</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>U34028673</t>
+          <t>U56204068</t>
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr">
         <is>
-          <t>82.50</t>
+          <t>91.19</t>
         </is>
       </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>
-          <t>15.10</t>
+          <t>37.34</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>82.50</t>
+          <t>91.19</t>
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr">
         <is>
-          <t>15.10</t>
+          <t>37.34</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>5444045</v>
+        <v>5446521</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1736,13 +1736,13 @@
         </is>
       </c>
       <c r="D21" s="2" t="n">
-        <v>45847.58949074074</v>
+        <v>45859.62079861111</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>2.537777777777778</v>
+        <v>3.548333333333333</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1751,42 +1751,42 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>CGS2100.002U25</t>
+          <t>CGS2100.021U25</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>U27804657</t>
+          <t>U34028673</t>
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
-          <t>89.97</t>
+          <t>79.69</t>
         </is>
       </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr">
         <is>
-          <t>19.19</t>
+          <t>22.72</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>89.97</t>
+          <t>79.69</t>
         </is>
       </c>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr">
         <is>
-          <t>19.19</t>
+          <t>22.72</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>5444997</v>
+        <v>5444045</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1799,13 +1799,13 @@
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>45849.62042824074</v>
+        <v>45859.60170138889</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>1.201111111111111</v>
+        <v>2.751111111111111</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1814,42 +1814,42 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>CGS2100.021U25</t>
+          <t>CGS2100.002U25</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>U87264562</t>
+          <t>U27804657</t>
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
-          <t>91.77</t>
+          <t>98.19</t>
         </is>
       </c>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr">
         <is>
-          <t>28.15</t>
+          <t>37.16</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>91.77</t>
+          <t>98.19</t>
         </is>
       </c>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr">
         <is>
-          <t>28.15</t>
+          <t>37.16</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>5435497</v>
+        <v>5444997</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1862,13 +1862,13 @@
         </is>
       </c>
       <c r="D23" s="2" t="n">
-        <v>45849.78327546296</v>
+        <v>45856.89804398148</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
-        <v>5.387222222222222</v>
+        <v>1.665277777777778</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1877,42 +1877,42 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>CGS2100.002U25</t>
+          <t>CGS2100.021U25</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>U41333662</t>
+          <t>U87264562</t>
         </is>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
-          <t>89.52</t>
+          <t>94.32</t>
         </is>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr">
         <is>
-          <t>23.55</t>
+          <t>27.42</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>89.52</t>
+          <t>94.32</t>
         </is>
       </c>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr">
         <is>
-          <t>23.55</t>
+          <t>27.42</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>5464229</v>
+        <v>5435497</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1925,13 +1925,13 @@
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>45848.38057870371</v>
+        <v>45859.62603009259</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>7.161388888888889</v>
+        <v>6.107222222222222</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1940,42 +1940,42 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>CGS2100.021U25</t>
+          <t>CGS2100.002U25</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>U31878090</t>
+          <t>U41333662</t>
         </is>
       </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
-          <t>97.69</t>
+          <t>89.52</t>
         </is>
       </c>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr">
         <is>
-          <t>32.00</t>
+          <t>27.30</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>97.69</t>
+          <t>89.52</t>
         </is>
       </c>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr">
         <is>
-          <t>32.00</t>
+          <t>27.30</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>5445225</v>
+        <v>5464229</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1988,13 +1988,13 @@
         </is>
       </c>
       <c r="D25" s="2" t="n">
-        <v>45849.56491898148</v>
+        <v>45859.63120370371</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>14.32333333333333</v>
+        <v>10.23027777777778</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -2008,37 +2008,37 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>U85513252</t>
+          <t>U31878090</t>
         </is>
       </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>99.13</t>
         </is>
       </c>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr">
         <is>
-          <t>16.40</t>
+          <t>39.97</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>85.92</t>
+          <t>99.13</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr">
         <is>
-          <t>16.40</t>
+          <t>39.97</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>5462855</v>
+        <v>5445225</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2051,13 +2051,13 @@
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>45847.63947916667</v>
+        <v>45856.12732638889</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
-        <v>10.78972222222222</v>
+        <v>19.24333333333333</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -2071,37 +2071,37 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>U04008596</t>
+          <t>U85513252</t>
         </is>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
-          <t>86.84</t>
+          <t>92.62</t>
         </is>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr">
         <is>
-          <t>18.00</t>
+          <t>25.24</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>86.84</t>
+          <t>92.62</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr">
         <is>
-          <t>18.00</t>
+          <t>25.24</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>5489989</v>
+        <v>5462855</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2114,13 +2114,13 @@
         </is>
       </c>
       <c r="D27" s="2" t="n">
-        <v>45848.92805555555</v>
+        <v>45859.62674768519</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>1.809166666666667</v>
+        <v>14.84055555555556</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -2134,37 +2134,37 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>U13049719</t>
+          <t>U04008596</t>
         </is>
       </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr">
         <is>
-          <t>85.13</t>
+          <t>100.00</t>
         </is>
       </c>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr">
         <is>
-          <t>16.10</t>
+          <t>31.42</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>85.13</t>
+          <t>100.00</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr">
         <is>
-          <t>16.10</t>
+          <t>31.42</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>5445015</v>
+        <v>5489989</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2177,13 +2177,13 @@
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>45849.78873842592</v>
+        <v>45859.57103009259</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>5.261944444444445</v>
+        <v>3.208888888888889</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -2192,42 +2192,42 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>CGS2100.002U25</t>
+          <t>CGS2100.021U25</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>U44650340</t>
+          <t>U13049719</t>
         </is>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
-          <t>97.04</t>
+          <t>93.09</t>
         </is>
       </c>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr">
         <is>
-          <t>32.83</t>
+          <t>28.19</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>97.04</t>
+          <t>93.09</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr">
         <is>
-          <t>32.83</t>
+          <t>28.19</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>5447619</v>
+        <v>5445015</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -2240,13 +2240,13 @@
         </is>
       </c>
       <c r="D29" s="2" t="n">
-        <v>45848.74439814815</v>
+        <v>45859.61010416667</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>4.226666666666667</v>
+        <v>8.452777777777778</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -2260,37 +2260,37 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>U34125866</t>
+          <t>U44650340</t>
         </is>
       </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
         <is>
-          <t>83.95</t>
+          <t>100.00</t>
         </is>
       </c>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr">
         <is>
-          <t>24.13</t>
+          <t>41.92</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>83.95</t>
+          <t>100.00</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr">
         <is>
-          <t>24.13</t>
+          <t>41.92</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>5425419</v>
+        <v>5447619</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -2303,13 +2303,13 @@
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>45849.73298611111</v>
+        <v>45859.55519675926</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>3.104722222222222</v>
+        <v>4.456666666666667</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -2323,37 +2323,37 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>U89866343</t>
+          <t>U34125866</t>
         </is>
       </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr">
         <is>
-          <t>86.23</t>
+          <t>87.03</t>
         </is>
       </c>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr">
         <is>
-          <t>17.77</t>
+          <t>21.70</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>86.23</t>
+          <t>87.03</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t>17.77</t>
+          <t>21.70</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>5509671</v>
+        <v>5425419</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2366,13 +2366,13 @@
         </is>
       </c>
       <c r="D31" s="2" t="n">
-        <v>45847.61751157408</v>
+        <v>45859.62236111111</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>2.414166666666667</v>
+        <v>6.120555555555556</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -2381,42 +2381,42 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>CGS2100.021U25</t>
+          <t>CGS2100.002U25</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>U33507894</t>
+          <t>U89866343</t>
         </is>
       </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
-          <t>86.93</t>
+          <t>96.80</t>
         </is>
       </c>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr">
         <is>
-          <t>16.78</t>
+          <t>28.98</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>86.93</t>
+          <t>96.80</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t>16.78</t>
+          <t>28.98</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>5441293</v>
+        <v>5509671</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -2429,13 +2429,13 @@
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>45849.77949074074</v>
+        <v>45859.6130787037</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>5.941388888888889</v>
+        <v>3.0425</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -2444,42 +2444,42 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>CGS2100.002U25</t>
+          <t>CGS2100.021U25</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>U24356879</t>
+          <t>U33507894</t>
         </is>
       </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr">
         <is>
-          <t>86.84</t>
+          <t>91.20</t>
         </is>
       </c>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr">
         <is>
-          <t>16.75</t>
+          <t>31.91</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>86.84</t>
+          <t>91.20</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t>16.75</t>
+          <t>31.91</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>5449907</v>
+        <v>5441293</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -2492,13 +2492,13 @@
         </is>
       </c>
       <c r="D33" s="2" t="n">
-        <v>45849.76997685185</v>
+        <v>45856.77885416667</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
-        <v>3.0925</v>
+        <v>6.860277777777778</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -2512,37 +2512,37 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>U08894019</t>
+          <t>U24356879</t>
         </is>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
-          <t>99.08</t>
+          <t>94.60</t>
         </is>
       </c>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr">
         <is>
-          <t>22.65</t>
+          <t>28.87</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>99.08</t>
+          <t>94.60</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr">
         <is>
-          <t>22.65</t>
+          <t>28.87</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>5488551</v>
+        <v>5449907</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -2555,13 +2555,13 @@
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>45849.69392361111</v>
+        <v>45859.60787037037</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>3.124444444444444</v>
+        <v>4.375555555555556</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -2575,37 +2575,37 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>U32417601</t>
+          <t>U08894019</t>
         </is>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
-          <t>80.97</t>
+          <t>97.29</t>
         </is>
       </c>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr">
         <is>
-          <t>14.52</t>
+          <t>46.99</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>80.97</t>
+          <t>97.29</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr">
         <is>
-          <t>14.52</t>
+          <t>46.99</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>5459463</v>
+        <v>5488551</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -2618,13 +2618,13 @@
         </is>
       </c>
       <c r="D35" s="2" t="n">
-        <v>45849.13179398148</v>
+        <v>45859.61040509259</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>1.784722222222222</v>
+        <v>7.597777777777778</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -2633,42 +2633,42 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>CGS2100.021U25</t>
+          <t>CGS2100.002U25</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>U44611120</t>
+          <t>U32417601</t>
         </is>
       </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr">
         <is>
-          <t>86.84</t>
+          <t>53.85</t>
         </is>
       </c>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr">
         <is>
-          <t>16.75</t>
+          <t>21.67</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>86.84</t>
+          <t>53.85</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr">
         <is>
-          <t>16.75</t>
+          <t>21.67</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>5501311</v>
+        <v>5459463</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -2681,13 +2681,13 @@
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>45848.21846064815</v>
+        <v>45859.62770833333</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>0.9350000000000001</v>
+        <v>2.261388888888889</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -2701,37 +2701,37 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>U75197896</t>
+          <t>U44611120</t>
         </is>
       </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr">
         <is>
-          <t>85.13</t>
+          <t>77.62</t>
         </is>
       </c>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr">
         <is>
-          <t>16.10</t>
+          <t>21.60</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>85.13</t>
+          <t>77.62</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr">
         <is>
-          <t>16.10</t>
+          <t>21.60</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>5445241</v>
+        <v>5501311</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -2744,13 +2744,13 @@
         </is>
       </c>
       <c r="D37" s="2" t="n">
-        <v>45847.83398148148</v>
+        <v>45859.62064814815</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>1.823333333333333</v>
+        <v>1.493333333333333</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -2764,37 +2764,37 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>U64836173</t>
+          <t>U75197896</t>
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr">
         <is>
-          <t>84.21</t>
+          <t>76.46</t>
         </is>
       </c>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr">
         <is>
-          <t>15.75</t>
+          <t>22.06</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>84.21</t>
+          <t>76.46</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr">
         <is>
-          <t>15.75</t>
+          <t>22.06</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>5458329</v>
+        <v>5445241</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -2807,13 +2807,13 @@
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>45848.97655092592</v>
+        <v>45859.62567129629</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>2.354444444444444</v>
+        <v>4.102222222222222</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -2827,37 +2827,37 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>U15555805</t>
+          <t>U64836173</t>
         </is>
       </c>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr">
         <is>
-          <t>78.95</t>
+          <t>90.15</t>
         </is>
       </c>
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr">
         <is>
-          <t>15.00</t>
+          <t>28.95</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>78.95</t>
+          <t>90.15</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr">
         <is>
-          <t>15.00</t>
+          <t>28.95</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>5487129</v>
+        <v>5458329</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -2870,13 +2870,13 @@
         </is>
       </c>
       <c r="D39" s="2" t="n">
-        <v>45847.82582175926</v>
+        <v>45859.60325231482</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>4.266666666666667</v>
+        <v>3.530277777777778</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -2890,37 +2890,37 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>U16616545</t>
+          <t>U15555805</t>
         </is>
       </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr">
         <is>
-          <t>90.32</t>
+          <t>71.91</t>
         </is>
       </c>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr">
         <is>
-          <t>31.93</t>
+          <t>22.10</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>90.32</t>
+          <t>71.91</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr">
         <is>
-          <t>31.93</t>
+          <t>22.10</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>5462903</v>
+        <v>5487129</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -2933,13 +2933,13 @@
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>45847.5974074074</v>
+        <v>45859.03394675926</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>1.709444444444445</v>
+        <v>6.205277777777778</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -2948,42 +2948,42 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>CGS2100.002U25</t>
+          <t>CGS2100.021U25</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>U74277121</t>
+          <t>U16616545</t>
         </is>
       </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr">
         <is>
-          <t>50.77</t>
+          <t>98.16</t>
         </is>
       </c>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr">
         <is>
-          <t>18.00</t>
+          <t>47.49</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>50.77</t>
+          <t>98.16</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr">
         <is>
-          <t>18.00</t>
+          <t>47.49</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>5459915</v>
+        <v>5462903</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -2996,13 +2996,13 @@
         </is>
       </c>
       <c r="D41" s="2" t="n">
-        <v>45849.06736111111</v>
+        <v>45859.57129629629</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>3.530555555555555</v>
+        <v>2.065277777777778</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -3011,42 +3011,42 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>CGS2100.021U25</t>
+          <t>CGS2100.002U25</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>U69599253</t>
+          <t>U74277121</t>
         </is>
       </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr">
         <is>
-          <t>82.50</t>
+          <t>92.82</t>
         </is>
       </c>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr">
         <is>
-          <t>15.10</t>
+          <t>25.30</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>82.50</t>
+          <t>92.82</t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr">
         <is>
-          <t>15.10</t>
+          <t>25.30</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>5445265</v>
+        <v>5459915</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -3059,13 +3059,13 @@
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>45848.78436342593</v>
+        <v>45859.60086805555</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>1.132777777777778</v>
+        <v>4.768333333333334</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -3079,37 +3079,37 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>U37563843</t>
+          <t>U69599253</t>
         </is>
       </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr">
         <is>
-          <t>82.50</t>
+          <t>89.85</t>
         </is>
       </c>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr">
         <is>
-          <t>15.10</t>
+          <t>23.45</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>82.50</t>
+          <t>89.85</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr">
         <is>
-          <t>15.10</t>
+          <t>23.45</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>5470105</v>
+        <v>5445265</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -3122,13 +3122,13 @@
         </is>
       </c>
       <c r="D43" s="2" t="n">
-        <v>45848.81870370371</v>
+        <v>45859.61564814814</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>2.523888888888889</v>
+        <v>1.882777777777778</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -3137,42 +3137,42 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>CGS2100.002U25</t>
+          <t>CGS2100.021U25</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>U14290608</t>
+          <t>U37563843</t>
         </is>
       </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr">
         <is>
-          <t>84.21</t>
+          <t>86.80</t>
         </is>
       </c>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr">
         <is>
-          <t>15.75</t>
+          <t>25.20</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>84.21</t>
+          <t>86.80</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr">
         <is>
-          <t>15.75</t>
+          <t>25.20</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>5447047</v>
+        <v>5470105</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -3185,13 +3185,13 @@
         </is>
       </c>
       <c r="D44" s="2" t="n">
-        <v>45849.78318287037</v>
+        <v>45859.62439814815</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>1.217777777777778</v>
+        <v>3.428055555555555</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -3205,37 +3205,37 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>U61622868</t>
+          <t>U14290608</t>
         </is>
       </c>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr">
         <is>
-          <t>84.30</t>
+          <t>90.77</t>
         </is>
       </c>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr">
         <is>
-          <t>15.78</t>
+          <t>24.25</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>84.30</t>
+          <t>90.77</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr">
         <is>
-          <t>15.78</t>
+          <t>24.25</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>5453441</v>
+        <v>5447047</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -3248,13 +3248,13 @@
         </is>
       </c>
       <c r="D45" s="2" t="n">
-        <v>45848.95607638889</v>
+        <v>45859.62346064814</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>2.141666666666667</v>
+        <v>3.480277777777778</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -3268,37 +3268,37 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>U78625911</t>
+          <t>U61622868</t>
         </is>
       </c>
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr">
         <is>
-          <t>93.49</t>
+          <t>73.57</t>
         </is>
       </c>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr">
         <is>
-          <t>29.27</t>
+          <t>21.01</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>93.49</t>
+          <t>73.57</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr">
         <is>
-          <t>29.27</t>
+          <t>21.01</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>5486665</v>
+        <v>5453441</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -3311,13 +3311,13 @@
         </is>
       </c>
       <c r="D46" s="2" t="n">
-        <v>45847.58957175926</v>
+        <v>45859.60914351852</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>2.976388888888889</v>
+        <v>2.516944444444444</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -3326,42 +3326,42 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>CGS2100.021U25</t>
+          <t>CGS2100.002U25</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>U95838760</t>
+          <t>U78625911</t>
         </is>
       </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr">
         <is>
-          <t>86.84</t>
+          <t>99.33</t>
         </is>
       </c>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr">
         <is>
-          <t>18.00</t>
+          <t>37.53</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>86.84</t>
+          <t>99.33</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr">
         <is>
-          <t>18.00</t>
+          <t>37.53</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>5461189</v>
+        <v>5486665</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -3374,13 +3374,13 @@
         </is>
       </c>
       <c r="D47" s="2" t="n">
-        <v>45849.19292824074</v>
+        <v>45859.62677083333</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>4.075277777777778</v>
+        <v>3.933611111111111</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -3389,42 +3389,42 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>CGS2100.002U25</t>
+          <t>CGS2100.021U25</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>U34392995</t>
+          <t>U95838760</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr">
         <is>
-          <t>77.63</t>
+          <t>82.34</t>
         </is>
       </c>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr">
         <is>
-          <t>13.25</t>
+          <t>24.80</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>77.63</t>
+          <t>82.34</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
       <c r="P47" t="inlineStr">
         <is>
-          <t>13.25</t>
+          <t>24.80</t>
         </is>
       </c>
       <c r="Q47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>5458119</v>
+        <v>5461189</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -3437,13 +3437,13 @@
         </is>
       </c>
       <c r="D48" s="2" t="n">
-        <v>45847.73429398148</v>
+        <v>45859.63163194444</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>2.046111111111111</v>
+        <v>5.495833333333334</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -3452,46 +3452,46 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>CGS2100.021U25</t>
+          <t>CGS2100.002U25</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>U52090888</t>
+          <t>U34392995</t>
         </is>
       </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr">
         <is>
-          <t>94.08</t>
+          <t>43.67</t>
         </is>
       </c>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr">
         <is>
-          <t>24.65</t>
+          <t>17.23</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>94.08</t>
+          <t>43.67</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr">
         <is>
-          <t>24.65</t>
+          <t>17.23</t>
         </is>
       </c>
       <c r="Q48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>5551489</v>
+        <v>5458119</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>StudentViewEnrollment</t>
+          <t>StudentEnrollment</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3500,13 +3500,13 @@
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>45845.59688657407</v>
+        <v>45859.59840277778</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>0.2288888888888889</v>
+        <v>3.129722222222222</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -3518,20 +3518,32 @@
           <t>CGS2100.021U25</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr"/>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>U52090888</t>
+        </is>
+      </c>
       <c r="J49" t="inlineStr"/>
-      <c r="K49" t="inlineStr"/>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>94.08</t>
+        </is>
+      </c>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr">
         <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="N49" t="inlineStr"/>
+          <t>25.90</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>94.08</t>
+        </is>
+      </c>
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>25.90</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr"/>
@@ -3554,7 +3566,7 @@
         <v>45845.59688657407</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F50" t="n">
         <v>0.2288888888888889</v>
@@ -3566,7 +3578,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>CGS2100.002U25</t>
+          <t>CGS2100.021U25</t>
         </is>
       </c>
       <c r="I50" t="inlineStr"/>
@@ -3589,26 +3601,26 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>5009103</v>
+        <v>5551489</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>TaEnrollment</t>
+          <t>StudentViewEnrollment</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>TaEnrollment</t>
+          <t>StudentEnrollment</t>
         </is>
       </c>
       <c r="D51" s="2" t="n">
-        <v>45845.69819444444</v>
+        <v>45845.59688657407</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F51" t="n">
-        <v>0.1555555555555556</v>
+        <v>0.2288888888888889</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -3620,23 +3632,27 @@
           <t>CGS2100.002U25</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>U88099159</t>
-        </is>
-      </c>
+      <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr"/>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr"/>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
       <c r="Q51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>4957763</v>
+        <v>5009103</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -3649,13 +3665,13 @@
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>45849.54942129629</v>
+        <v>45849.85122685185</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
-        <v>0.03583333333333334</v>
+        <v>0.1555555555555556</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -3669,7 +3685,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>U64219048</t>
+          <t>U88099159</t>
         </is>
       </c>
       <c r="J52" t="inlineStr"/>
@@ -3683,7 +3699,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>4876881</v>
+        <v>4957763</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -3696,13 +3712,13 @@
         </is>
       </c>
       <c r="D53" s="2" t="n">
-        <v>45849.80597222222</v>
+        <v>45857.78738425926</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>0.4030555555555556</v>
+        <v>0.3816666666666667</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -3716,7 +3732,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>U14884292</t>
+          <t>U64219048</t>
         </is>
       </c>
       <c r="J53" t="inlineStr"/>
@@ -3730,7 +3746,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>5106229</v>
+        <v>4876881</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -3743,13 +3759,13 @@
         </is>
       </c>
       <c r="D54" s="2" t="n">
-        <v>45846.71395833333</v>
+        <v>45859.63210648148</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>0.1425</v>
+        <v>0.6830555555555555</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -3763,7 +3779,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>U95564252</t>
+          <t>U14884292</t>
         </is>
       </c>
       <c r="J54" t="inlineStr"/>
@@ -3777,7 +3793,7 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>5061721</v>
+        <v>5106229</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -3789,10 +3805,14 @@
           <t>TaEnrollment</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
+      <c r="D55" s="2" t="n">
+        <v>45858.99600694444</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
       <c r="F55" t="n">
-        <v>0</v>
+        <v>0.195</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -3806,7 +3826,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>U34561707</t>
+          <t>U95564252</t>
         </is>
       </c>
       <c r="J55" t="inlineStr"/>
@@ -3820,26 +3840,22 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>964585</v>
+        <v>5061721</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>TeacherEnrollment</t>
+          <t>TaEnrollment</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>TeacherEnrollment</t>
-        </is>
-      </c>
-      <c r="D56" s="2" t="n">
-        <v>45847.59443287037</v>
-      </c>
-      <c r="E56" t="n">
-        <v>2</v>
-      </c>
+          <t>TaEnrollment</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr"/>
       <c r="F56" t="n">
-        <v>5.233055555555556</v>
+        <v>0</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -3853,7 +3869,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>U84383097</t>
+          <t>U34561707</t>
         </is>
       </c>
       <c r="J56" t="inlineStr"/>
@@ -3880,13 +3896,13 @@
         </is>
       </c>
       <c r="D57" s="2" t="n">
-        <v>45847.59443287037</v>
+        <v>45859.5621875</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>5.233055555555556</v>
+        <v>6.229722222222223</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -3895,7 +3911,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>CGS2100.021U25</t>
+          <t>CGS2100.002U25</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -3912,6 +3928,53 @@
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="inlineStr"/>
     </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>964585</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>TeacherEnrollment</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>TeacherEnrollment</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>45859.5621875</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>6.229722222222223</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>CGS2100.002U25</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>CGS2100.021U25</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>U84383097</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>